<commit_message>
[dev] Add all structure
</commit_message>
<xml_diff>
--- a/LocalDertyu.xlsx
+++ b/LocalDertyu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ML-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7523EE9-945B-4DE0-A245-DB32BCD99DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBE2CE9-D02F-4D05-B8BE-8DA334374E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
   <si>
     <t>Learning rate</t>
   </si>
@@ -67,6 +67,69 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>0.001</t>
+  </si>
+  <si>
+    <t>ReLU</t>
+  </si>
+  <si>
+    <t>3, 2</t>
+  </si>
+  <si>
+    <t>48х48</t>
+  </si>
+  <si>
+    <t>VGG v1.1</t>
+  </si>
+  <si>
+    <t>VGG v1.2</t>
+  </si>
+  <si>
+    <t>RELU</t>
+  </si>
+  <si>
+    <t>48x48</t>
+  </si>
+  <si>
+    <t>VGG v1.3</t>
+  </si>
+  <si>
+    <t>64x64</t>
+  </si>
+  <si>
+    <t>Лучшая</t>
+  </si>
+  <si>
+    <t>VGG v1.4</t>
+  </si>
+  <si>
+    <t>35(15-20)</t>
+  </si>
+  <si>
+    <t>Optimizer</t>
+  </si>
+  <si>
+    <t>Linear layers count</t>
+  </si>
+  <si>
+    <t>__</t>
+  </si>
+  <si>
+    <t>CE</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>Augmentations</t>
+  </si>
+  <si>
+    <t>Function Loss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RHF(0.5), RR(10), RVF(0.5), CJ(0.2, 0.2, 0.2, 0.1) </t>
   </si>
 </sst>
 </file>
@@ -121,13 +184,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -415,47 +482,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="Q2" sqref="A2:Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
     <col min="4" max="4" width="26.85546875" customWidth="1"/>
     <col min="5" max="5" width="21.5703125" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" customWidth="1"/>
     <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" customWidth="1"/>
     <col min="9" max="9" width="16.42578125" customWidth="1"/>
     <col min="10" max="10" width="14.140625" customWidth="1"/>
     <col min="11" max="11" width="13.85546875" customWidth="1"/>
     <col min="12" max="12" width="13.140625" customWidth="1"/>
     <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" customWidth="1"/>
+    <col min="16" max="16" width="18.7109375" customWidth="1"/>
+    <col min="17" max="17" width="43.28515625" customWidth="1"/>
     <col min="18" max="18" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4" t="s">
+    <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -494,13 +570,228 @@
       </c>
       <c r="M2" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>45626</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>9</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3">
+        <v>8</v>
+      </c>
+      <c r="L3">
+        <v>3</v>
+      </c>
+      <c r="N3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>45627</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4">
+        <v>8</v>
+      </c>
+      <c r="L4">
+        <v>10</v>
+      </c>
+      <c r="N4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" t="s">
+        <v>30</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>45627</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>6</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5">
+        <v>16</v>
+      </c>
+      <c r="L5">
+        <v>10</v>
+      </c>
+      <c r="N5" t="s">
+        <v>31</v>
+      </c>
+      <c r="O5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>45627</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6">
+        <v>24</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" t="s">
+        <v>31</v>
+      </c>
+      <c r="O6" t="s">
+        <v>30</v>
+      </c>
+      <c r="P6">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="R6" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="J1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>